<commit_message>
0.56 ready for level 3 room development
</commit_message>
<xml_diff>
--- a/src/main/screeps.xlsx
+++ b/src/main/screeps.xlsx
@@ -8,12 +8,13 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Screeps\screeps-kotlin-starter-master\src\main\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{279D5F9B-0236-4266-945D-90407B7709F7}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CBFDA2AE-C64F-4BF8-93D8-F10EDC67C2FA}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{E64D4CD0-F693-495E-97B0-F1DF3284CC0F}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{E64D4CD0-F693-495E-97B0-F1DF3284CC0F}"/>
   </bookViews>
   <sheets>
-    <sheet name="Лист1" sheetId="1" r:id="rId1"/>
+    <sheet name="plan expansion" sheetId="1" r:id="rId1"/>
+    <sheet name="lab" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -30,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="193" uniqueCount="88">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="199" uniqueCount="94">
   <si>
     <t>O</t>
   </si>
@@ -294,6 +295,24 @@
   </si>
   <si>
     <t>E57N32</t>
+  </si>
+  <si>
+    <t>lvl</t>
+  </si>
+  <si>
+    <t>last for upgraids</t>
+  </si>
+  <si>
+    <t>2. перебором относительно minX, minY определяем номер labs</t>
+  </si>
+  <si>
+    <t>example lab2 = minX+2,minY</t>
+  </si>
+  <si>
+    <t>Aloritm to find a number of labs</t>
+  </si>
+  <si>
+    <t>1. Find minX, minY all labs</t>
   </si>
 </sst>
 </file>
@@ -325,7 +344,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="10">
+  <fills count="11">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -377,6 +396,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FF00B050"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -445,7 +470,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="15">
+  <cellXfs count="18">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
@@ -455,6 +480,11 @@
     </xf>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="7" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="8" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -464,11 +494,9 @@
     <xf numFmtId="0" fontId="1" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="7" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="8" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="10" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Обычный" xfId="0" builtinId="0"/>
@@ -790,8 +818,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BAF91D9F-DCEA-4E79-967A-CDC2E1F2774F}">
   <dimension ref="D3:AZ32"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="AC20" sqref="AC20"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="Z28" sqref="Z28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -851,51 +879,51 @@
         <v>6</v>
       </c>
       <c r="Y4" s="2"/>
-      <c r="Z4" s="7" t="s">
+      <c r="Z4" s="12" t="s">
         <v>37</v>
       </c>
-      <c r="AA4" s="8"/>
-      <c r="AB4" s="9"/>
-      <c r="AC4" s="7" t="s">
+      <c r="AA4" s="13"/>
+      <c r="AB4" s="14"/>
+      <c r="AC4" s="12" t="s">
         <v>38</v>
       </c>
-      <c r="AD4" s="8"/>
-      <c r="AE4" s="9"/>
-      <c r="AF4" s="7" t="s">
+      <c r="AD4" s="13"/>
+      <c r="AE4" s="14"/>
+      <c r="AF4" s="12" t="s">
         <v>39</v>
       </c>
-      <c r="AG4" s="8"/>
-      <c r="AH4" s="9"/>
-      <c r="AI4" s="7" t="s">
+      <c r="AG4" s="13"/>
+      <c r="AH4" s="14"/>
+      <c r="AI4" s="12" t="s">
         <v>40</v>
       </c>
-      <c r="AJ4" s="8"/>
-      <c r="AK4" s="9"/>
-      <c r="AL4" s="7" t="s">
+      <c r="AJ4" s="13"/>
+      <c r="AK4" s="14"/>
+      <c r="AL4" s="12" t="s">
         <v>41</v>
       </c>
-      <c r="AM4" s="8"/>
-      <c r="AN4" s="9"/>
-      <c r="AO4" s="7" t="s">
+      <c r="AM4" s="13"/>
+      <c r="AN4" s="14"/>
+      <c r="AO4" s="12" t="s">
         <v>42</v>
       </c>
-      <c r="AP4" s="8"/>
-      <c r="AQ4" s="9"/>
-      <c r="AR4" s="7" t="s">
+      <c r="AP4" s="13"/>
+      <c r="AQ4" s="14"/>
+      <c r="AR4" s="12" t="s">
         <v>43</v>
       </c>
-      <c r="AS4" s="8"/>
-      <c r="AT4" s="9"/>
-      <c r="AU4" s="7" t="s">
+      <c r="AS4" s="13"/>
+      <c r="AT4" s="14"/>
+      <c r="AU4" s="12" t="s">
         <v>44</v>
       </c>
-      <c r="AV4" s="8"/>
-      <c r="AW4" s="9"/>
-      <c r="AX4" s="7" t="s">
+      <c r="AV4" s="13"/>
+      <c r="AW4" s="14"/>
+      <c r="AX4" s="12" t="s">
         <v>45</v>
       </c>
-      <c r="AY4" s="8"/>
-      <c r="AZ4" s="9"/>
+      <c r="AY4" s="13"/>
+      <c r="AZ4" s="14"/>
     </row>
     <row r="5" spans="4:52" x14ac:dyDescent="0.25">
       <c r="D5">
@@ -940,77 +968,77 @@
       <c r="Y5" s="3" t="s">
         <v>46</v>
       </c>
-      <c r="Z5" s="12">
-        <v>2</v>
-      </c>
-      <c r="AA5" s="12" t="s">
+      <c r="Z5" s="9">
+        <v>2</v>
+      </c>
+      <c r="AA5" s="9" t="s">
         <v>0</v>
       </c>
-      <c r="AB5" s="12" t="s">
+      <c r="AB5" s="9" t="s">
         <v>64</v>
       </c>
-      <c r="AC5" s="11">
-        <v>1</v>
-      </c>
-      <c r="AD5" s="11" t="s">
+      <c r="AC5" s="8">
+        <v>1</v>
+      </c>
+      <c r="AD5" s="8" t="s">
         <v>0</v>
       </c>
-      <c r="AE5" s="11" t="s">
+      <c r="AE5" s="8" t="s">
         <v>62</v>
       </c>
-      <c r="AF5" s="12">
-        <v>2</v>
-      </c>
-      <c r="AG5" s="12" t="s">
-        <v>1</v>
-      </c>
-      <c r="AH5" s="12" t="s">
+      <c r="AF5" s="9">
+        <v>2</v>
+      </c>
+      <c r="AG5" s="9" t="s">
+        <v>1</v>
+      </c>
+      <c r="AH5" s="9" t="s">
         <v>64</v>
       </c>
-      <c r="AI5" s="12">
-        <v>2</v>
-      </c>
-      <c r="AJ5" s="12" t="s">
-        <v>2</v>
-      </c>
-      <c r="AK5" s="12" t="s">
+      <c r="AI5" s="9">
+        <v>2</v>
+      </c>
+      <c r="AJ5" s="9" t="s">
+        <v>2</v>
+      </c>
+      <c r="AK5" s="9" t="s">
         <v>64</v>
       </c>
       <c r="AL5" s="5"/>
       <c r="AM5" s="5"/>
       <c r="AN5" s="5"/>
-      <c r="AO5" s="13">
-        <v>2</v>
-      </c>
-      <c r="AP5" s="13" t="s">
-        <v>1</v>
-      </c>
-      <c r="AQ5" s="13" t="s">
+      <c r="AO5" s="10">
+        <v>2</v>
+      </c>
+      <c r="AP5" s="10" t="s">
+        <v>1</v>
+      </c>
+      <c r="AQ5" s="10" t="s">
         <v>62</v>
       </c>
-      <c r="AR5" s="10">
-        <v>1</v>
-      </c>
-      <c r="AS5" s="10" t="s">
+      <c r="AR5" s="7">
+        <v>1</v>
+      </c>
+      <c r="AS5" s="7" t="s">
         <v>4</v>
       </c>
-      <c r="AT5" s="10" t="s">
+      <c r="AT5" s="7" t="s">
         <v>68</v>
       </c>
-      <c r="AU5" s="10">
-        <v>1</v>
-      </c>
-      <c r="AV5" s="10" t="s">
-        <v>2</v>
-      </c>
-      <c r="AW5" s="10"/>
-      <c r="AX5" s="13">
-        <v>1</v>
-      </c>
-      <c r="AY5" s="13" t="s">
-        <v>1</v>
-      </c>
-      <c r="AZ5" s="13" t="s">
+      <c r="AU5" s="7">
+        <v>1</v>
+      </c>
+      <c r="AV5" s="7" t="s">
+        <v>2</v>
+      </c>
+      <c r="AW5" s="7"/>
+      <c r="AX5" s="10">
+        <v>1</v>
+      </c>
+      <c r="AY5" s="10" t="s">
+        <v>1</v>
+      </c>
+      <c r="AZ5" s="10" t="s">
         <v>75</v>
       </c>
     </row>
@@ -1055,77 +1083,77 @@
       <c r="Y6" s="2" t="s">
         <v>47</v>
       </c>
-      <c r="Z6" s="11">
-        <v>1</v>
-      </c>
-      <c r="AA6" s="11" t="s">
+      <c r="Z6" s="8">
+        <v>1</v>
+      </c>
+      <c r="AA6" s="8" t="s">
         <v>5</v>
       </c>
-      <c r="AB6" s="11" t="s">
+      <c r="AB6" s="8" t="s">
         <v>63</v>
       </c>
-      <c r="AC6" s="12">
-        <v>2</v>
-      </c>
-      <c r="AD6" s="12" t="s">
-        <v>2</v>
-      </c>
-      <c r="AE6" s="12" t="s">
+      <c r="AC6" s="9">
+        <v>2</v>
+      </c>
+      <c r="AD6" s="9" t="s">
+        <v>2</v>
+      </c>
+      <c r="AE6" s="9" t="s">
         <v>66</v>
       </c>
-      <c r="AF6" s="12">
-        <v>2</v>
-      </c>
-      <c r="AG6" s="12" t="s">
+      <c r="AF6" s="9">
+        <v>2</v>
+      </c>
+      <c r="AG6" s="9" t="s">
         <v>0</v>
       </c>
-      <c r="AH6" s="12"/>
-      <c r="AI6" s="11">
-        <v>1</v>
-      </c>
-      <c r="AJ6" s="11" t="s">
-        <v>2</v>
-      </c>
-      <c r="AK6" s="11" t="s">
+      <c r="AH6" s="9"/>
+      <c r="AI6" s="8">
+        <v>1</v>
+      </c>
+      <c r="AJ6" s="8" t="s">
+        <v>2</v>
+      </c>
+      <c r="AK6" s="8" t="s">
         <v>63</v>
       </c>
       <c r="AL6" s="5"/>
       <c r="AM6" s="5"/>
       <c r="AN6" s="5"/>
-      <c r="AO6" s="13">
-        <v>1</v>
-      </c>
-      <c r="AP6" s="13" t="s">
-        <v>1</v>
-      </c>
-      <c r="AQ6" s="13" t="s">
+      <c r="AO6" s="10">
+        <v>1</v>
+      </c>
+      <c r="AP6" s="10" t="s">
+        <v>1</v>
+      </c>
+      <c r="AQ6" s="10" t="s">
         <v>62</v>
       </c>
-      <c r="AR6" s="13">
-        <v>1</v>
-      </c>
-      <c r="AS6" s="13" t="s">
+      <c r="AR6" s="10">
+        <v>1</v>
+      </c>
+      <c r="AS6" s="10" t="s">
         <v>0</v>
       </c>
-      <c r="AT6" s="13" t="s">
+      <c r="AT6" s="10" t="s">
         <v>63</v>
       </c>
-      <c r="AU6" s="13">
-        <v>1</v>
-      </c>
-      <c r="AV6" s="13" t="s">
+      <c r="AU6" s="10">
+        <v>1</v>
+      </c>
+      <c r="AV6" s="10" t="s">
         <v>0</v>
       </c>
-      <c r="AW6" s="13" t="s">
+      <c r="AW6" s="10" t="s">
         <v>75</v>
       </c>
-      <c r="AX6" s="12">
-        <v>2</v>
-      </c>
-      <c r="AY6" s="12" t="s">
-        <v>2</v>
-      </c>
-      <c r="AZ6" s="12" t="s">
+      <c r="AX6" s="9">
+        <v>2</v>
+      </c>
+      <c r="AY6" s="9" t="s">
+        <v>2</v>
+      </c>
+      <c r="AZ6" s="9" t="s">
         <v>65</v>
       </c>
     </row>
@@ -1170,40 +1198,40 @@
       <c r="Y7" s="3" t="s">
         <v>48</v>
       </c>
-      <c r="Z7" s="12">
-        <v>2</v>
-      </c>
-      <c r="AA7" s="12" t="s">
+      <c r="Z7" s="9">
+        <v>2</v>
+      </c>
+      <c r="AA7" s="9" t="s">
         <v>5</v>
       </c>
-      <c r="AB7" s="12" t="s">
+      <c r="AB7" s="9" t="s">
         <v>66</v>
       </c>
-      <c r="AC7" s="12">
-        <v>2</v>
-      </c>
-      <c r="AD7" s="12" t="s">
+      <c r="AC7" s="9">
+        <v>2</v>
+      </c>
+      <c r="AD7" s="9" t="s">
         <v>5</v>
       </c>
-      <c r="AE7" s="12" t="s">
+      <c r="AE7" s="9" t="s">
         <v>66</v>
       </c>
-      <c r="AF7" s="11">
-        <v>1</v>
-      </c>
-      <c r="AG7" s="11" t="s">
+      <c r="AF7" s="8">
+        <v>1</v>
+      </c>
+      <c r="AG7" s="8" t="s">
         <v>0</v>
       </c>
-      <c r="AH7" s="11" t="s">
+      <c r="AH7" s="8" t="s">
         <v>62</v>
       </c>
-      <c r="AI7" s="12">
-        <v>2</v>
-      </c>
-      <c r="AJ7" s="12" t="s">
+      <c r="AI7" s="9">
+        <v>2</v>
+      </c>
+      <c r="AJ7" s="9" t="s">
         <v>0</v>
       </c>
-      <c r="AK7" s="12" t="s">
+      <c r="AK7" s="9" t="s">
         <v>65</v>
       </c>
       <c r="AL7" s="5"/>
@@ -1212,31 +1240,31 @@
       <c r="AO7" s="5"/>
       <c r="AP7" s="5"/>
       <c r="AQ7" s="5"/>
-      <c r="AR7" s="10">
-        <v>1</v>
-      </c>
-      <c r="AS7" s="10" t="s">
+      <c r="AR7" s="7">
+        <v>1</v>
+      </c>
+      <c r="AS7" s="7" t="s">
         <v>0</v>
       </c>
-      <c r="AT7" s="10" t="s">
+      <c r="AT7" s="7" t="s">
         <v>65</v>
       </c>
-      <c r="AU7" s="10">
-        <v>2</v>
-      </c>
-      <c r="AV7" s="10" t="s">
+      <c r="AU7" s="7">
+        <v>2</v>
+      </c>
+      <c r="AV7" s="7" t="s">
         <v>0</v>
       </c>
-      <c r="AW7" s="10" t="s">
+      <c r="AW7" s="7" t="s">
         <v>64</v>
       </c>
-      <c r="AX7" s="13">
-        <v>1</v>
-      </c>
-      <c r="AY7" s="13" t="s">
+      <c r="AX7" s="10">
+        <v>1</v>
+      </c>
+      <c r="AY7" s="10" t="s">
         <v>0</v>
       </c>
-      <c r="AZ7" s="13" t="s">
+      <c r="AZ7" s="10" t="s">
         <v>63</v>
       </c>
     </row>
@@ -1282,79 +1310,79 @@
       <c r="Y8" s="2" t="s">
         <v>49</v>
       </c>
-      <c r="Z8" s="13">
-        <v>1</v>
-      </c>
-      <c r="AA8" s="13" t="s">
+      <c r="Z8" s="10">
+        <v>1</v>
+      </c>
+      <c r="AA8" s="10" t="s">
         <v>4</v>
       </c>
-      <c r="AB8" s="13" t="s">
+      <c r="AB8" s="10" t="s">
         <v>62</v>
       </c>
-      <c r="AC8" s="10">
-        <v>1</v>
-      </c>
-      <c r="AD8" s="10" t="s">
+      <c r="AC8" s="7">
+        <v>1</v>
+      </c>
+      <c r="AD8" s="7" t="s">
         <v>6</v>
       </c>
-      <c r="AE8" s="10" t="s">
+      <c r="AE8" s="7" t="s">
         <v>74</v>
       </c>
-      <c r="AF8" s="13">
-        <v>1</v>
-      </c>
-      <c r="AG8" s="13" t="s">
+      <c r="AF8" s="10">
+        <v>1</v>
+      </c>
+      <c r="AG8" s="10" t="s">
         <v>4</v>
       </c>
-      <c r="AH8" s="13" t="s">
+      <c r="AH8" s="10" t="s">
         <v>67</v>
       </c>
-      <c r="AI8" s="13">
+      <c r="AI8" s="10">
         <v>3</v>
       </c>
-      <c r="AJ8" s="13" t="s">
+      <c r="AJ8" s="10" t="s">
         <v>4</v>
       </c>
-      <c r="AK8" s="13" t="s">
+      <c r="AK8" s="10" t="s">
         <v>63</v>
       </c>
       <c r="AL8" s="6"/>
       <c r="AM8" s="6"/>
       <c r="AN8" s="6"/>
-      <c r="AO8" s="13">
+      <c r="AO8" s="10">
         <v>3</v>
       </c>
-      <c r="AP8" s="13" t="s">
-        <v>1</v>
-      </c>
-      <c r="AQ8" s="13" t="s">
+      <c r="AP8" s="10" t="s">
+        <v>1</v>
+      </c>
+      <c r="AQ8" s="10" t="s">
         <v>62</v>
       </c>
-      <c r="AR8" s="13">
-        <v>1</v>
-      </c>
-      <c r="AS8" s="13" t="s">
-        <v>2</v>
-      </c>
-      <c r="AT8" s="13" t="s">
+      <c r="AR8" s="10">
+        <v>1</v>
+      </c>
+      <c r="AS8" s="10" t="s">
+        <v>2</v>
+      </c>
+      <c r="AT8" s="10" t="s">
         <v>63</v>
       </c>
-      <c r="AU8" s="11">
-        <v>1</v>
-      </c>
-      <c r="AV8" s="11" t="s">
+      <c r="AU8" s="8">
+        <v>1</v>
+      </c>
+      <c r="AV8" s="8" t="s">
         <v>0</v>
       </c>
-      <c r="AW8" s="11" t="s">
+      <c r="AW8" s="8" t="s">
         <v>62</v>
       </c>
-      <c r="AX8" s="12">
-        <v>2</v>
-      </c>
-      <c r="AY8" s="12" t="s">
-        <v>1</v>
-      </c>
-      <c r="AZ8" s="12" t="s">
+      <c r="AX8" s="9">
+        <v>2</v>
+      </c>
+      <c r="AY8" s="9" t="s">
+        <v>1</v>
+      </c>
+      <c r="AZ8" s="9" t="s">
         <v>64</v>
       </c>
     </row>
@@ -1399,22 +1427,22 @@
       <c r="Y9" s="3" t="s">
         <v>50</v>
       </c>
-      <c r="Z9" s="10">
-        <v>2</v>
-      </c>
-      <c r="AA9" s="10" t="s">
+      <c r="Z9" s="7">
+        <v>2</v>
+      </c>
+      <c r="AA9" s="7" t="s">
         <v>5</v>
       </c>
-      <c r="AB9" s="10" t="s">
+      <c r="AB9" s="7" t="s">
         <v>64</v>
       </c>
-      <c r="AC9" s="12">
-        <v>2</v>
-      </c>
-      <c r="AD9" s="12" t="s">
+      <c r="AC9" s="9">
+        <v>2</v>
+      </c>
+      <c r="AD9" s="9" t="s">
         <v>5</v>
       </c>
-      <c r="AE9" s="12" t="s">
+      <c r="AE9" s="9" t="s">
         <v>64</v>
       </c>
       <c r="AF9" s="5"/>
@@ -1426,40 +1454,40 @@
       <c r="AL9" s="5"/>
       <c r="AM9" s="5"/>
       <c r="AN9" s="5"/>
-      <c r="AO9" s="13">
+      <c r="AO9" s="10">
         <v>3</v>
       </c>
-      <c r="AP9" s="13" t="s">
-        <v>1</v>
-      </c>
-      <c r="AQ9" s="13" t="s">
+      <c r="AP9" s="10" t="s">
+        <v>1</v>
+      </c>
+      <c r="AQ9" s="10" t="s">
         <v>62</v>
       </c>
-      <c r="AR9" s="10">
-        <v>1</v>
-      </c>
-      <c r="AS9" s="10" t="s">
-        <v>2</v>
-      </c>
-      <c r="AT9" s="10" t="s">
+      <c r="AR9" s="7">
+        <v>1</v>
+      </c>
+      <c r="AS9" s="7" t="s">
+        <v>2</v>
+      </c>
+      <c r="AT9" s="7" t="s">
         <v>68</v>
       </c>
-      <c r="AU9" s="13">
-        <v>1</v>
-      </c>
-      <c r="AV9" s="13" t="s">
-        <v>2</v>
-      </c>
-      <c r="AW9" s="13" t="s">
+      <c r="AU9" s="10">
+        <v>1</v>
+      </c>
+      <c r="AV9" s="10" t="s">
+        <v>2</v>
+      </c>
+      <c r="AW9" s="10" t="s">
         <v>67</v>
       </c>
-      <c r="AX9" s="13">
-        <v>1</v>
-      </c>
-      <c r="AY9" s="13" t="s">
+      <c r="AX9" s="10">
+        <v>1</v>
+      </c>
+      <c r="AY9" s="10" t="s">
         <v>5</v>
       </c>
-      <c r="AZ9" s="13" t="s">
+      <c r="AZ9" s="10" t="s">
         <v>67</v>
       </c>
     </row>
@@ -1500,22 +1528,22 @@
       <c r="Y10" s="2" t="s">
         <v>51</v>
       </c>
-      <c r="Z10" s="13">
-        <v>1</v>
-      </c>
-      <c r="AA10" s="13" t="s">
-        <v>1</v>
-      </c>
-      <c r="AB10" s="13" t="s">
+      <c r="Z10" s="10">
+        <v>1</v>
+      </c>
+      <c r="AA10" s="10" t="s">
+        <v>1</v>
+      </c>
+      <c r="AB10" s="10" t="s">
         <v>63</v>
       </c>
-      <c r="AC10" s="13">
-        <v>1</v>
-      </c>
-      <c r="AD10" s="13" t="s">
+      <c r="AC10" s="10">
+        <v>1</v>
+      </c>
+      <c r="AD10" s="10" t="s">
         <v>5</v>
       </c>
-      <c r="AE10" s="13" t="s">
+      <c r="AE10" s="10" t="s">
         <v>63</v>
       </c>
       <c r="AF10" s="5"/>
@@ -1527,22 +1555,22 @@
       <c r="AL10" s="5"/>
       <c r="AM10" s="5"/>
       <c r="AN10" s="5"/>
-      <c r="AO10" s="13">
+      <c r="AO10" s="10">
         <v>3</v>
       </c>
-      <c r="AP10" s="13" t="s">
+      <c r="AP10" s="10" t="s">
         <v>0</v>
       </c>
-      <c r="AQ10" s="13" t="s">
+      <c r="AQ10" s="10" t="s">
         <v>62</v>
       </c>
-      <c r="AR10" s="12">
-        <v>2</v>
-      </c>
-      <c r="AS10" s="12" t="s">
+      <c r="AR10" s="9">
+        <v>2</v>
+      </c>
+      <c r="AS10" s="9" t="s">
         <v>0</v>
       </c>
-      <c r="AT10" s="12" t="s">
+      <c r="AT10" s="9" t="s">
         <v>64</v>
       </c>
       <c r="AU10" s="5"/>
@@ -1594,20 +1622,20 @@
       <c r="Y11" s="3" t="s">
         <v>52</v>
       </c>
-      <c r="Z11" s="10">
-        <v>2</v>
-      </c>
-      <c r="AA11" s="10" t="s">
+      <c r="Z11" s="7">
+        <v>2</v>
+      </c>
+      <c r="AA11" s="7" t="s">
         <v>5</v>
       </c>
-      <c r="AB11" s="10"/>
-      <c r="AC11" s="10">
-        <v>1</v>
-      </c>
-      <c r="AD11" s="10" t="s">
+      <c r="AB11" s="7"/>
+      <c r="AC11" s="7">
+        <v>1</v>
+      </c>
+      <c r="AD11" s="7" t="s">
         <v>3</v>
       </c>
-      <c r="AE11" s="10"/>
+      <c r="AE11" s="7"/>
       <c r="AF11" s="5"/>
       <c r="AG11" s="5"/>
       <c r="AH11" s="5"/>
@@ -1617,22 +1645,22 @@
       <c r="AL11" s="5"/>
       <c r="AM11" s="5"/>
       <c r="AN11" s="5"/>
-      <c r="AO11" s="13">
-        <v>1</v>
-      </c>
-      <c r="AP11" s="13" t="s">
+      <c r="AO11" s="10">
+        <v>1</v>
+      </c>
+      <c r="AP11" s="10" t="s">
         <v>0</v>
       </c>
-      <c r="AQ11" s="13" t="s">
+      <c r="AQ11" s="10" t="s">
         <v>62</v>
       </c>
-      <c r="AR11" s="13">
-        <v>2</v>
-      </c>
-      <c r="AS11" s="13" t="s">
+      <c r="AR11" s="10">
+        <v>2</v>
+      </c>
+      <c r="AS11" s="10" t="s">
         <v>0</v>
       </c>
-      <c r="AT11" s="13" t="s">
+      <c r="AT11" s="10" t="s">
         <v>75</v>
       </c>
       <c r="AU11" s="5"/>
@@ -1686,22 +1714,22 @@
       <c r="AL12" s="5"/>
       <c r="AM12" s="5"/>
       <c r="AN12" s="5"/>
-      <c r="AO12" s="13">
-        <v>1</v>
-      </c>
-      <c r="AP12" s="13" t="s">
+      <c r="AO12" s="10">
+        <v>1</v>
+      </c>
+      <c r="AP12" s="10" t="s">
         <v>5</v>
       </c>
-      <c r="AQ12" s="13" t="s">
+      <c r="AQ12" s="10" t="s">
         <v>75</v>
       </c>
-      <c r="AR12" s="10">
-        <v>2</v>
-      </c>
-      <c r="AS12" s="10" t="s">
+      <c r="AR12" s="7">
+        <v>2</v>
+      </c>
+      <c r="AS12" s="7" t="s">
         <v>4</v>
       </c>
-      <c r="AT12" s="10" t="s">
+      <c r="AT12" s="7" t="s">
         <v>65</v>
       </c>
       <c r="AU12" s="5"/>
@@ -1755,22 +1783,22 @@
       <c r="AL13" s="5"/>
       <c r="AM13" s="5"/>
       <c r="AN13" s="5"/>
-      <c r="AO13" s="10">
-        <v>1</v>
-      </c>
-      <c r="AP13" s="10" t="s">
+      <c r="AO13" s="7">
+        <v>1</v>
+      </c>
+      <c r="AP13" s="7" t="s">
         <v>6</v>
       </c>
-      <c r="AQ13" s="10" t="s">
+      <c r="AQ13" s="7" t="s">
         <v>65</v>
       </c>
-      <c r="AR13" s="13">
-        <v>1</v>
-      </c>
-      <c r="AS13" s="13" t="s">
+      <c r="AR13" s="10">
+        <v>1</v>
+      </c>
+      <c r="AS13" s="10" t="s">
         <v>5</v>
       </c>
-      <c r="AT13" s="13" t="s">
+      <c r="AT13" s="10" t="s">
         <v>67</v>
       </c>
       <c r="AU13" s="5"/>
@@ -1877,10 +1905,10 @@
       <c r="M17" s="2">
         <v>1</v>
       </c>
-      <c r="N17" s="14" t="s">
+      <c r="N17" s="11" t="s">
         <v>78</v>
       </c>
-      <c r="O17" s="14" t="s">
+      <c r="O17" s="11" t="s">
         <v>77</v>
       </c>
       <c r="P17" s="2"/>
@@ -1953,10 +1981,10 @@
       <c r="K20" s="3"/>
       <c r="L20" s="3"/>
       <c r="M20" s="3"/>
-      <c r="N20" s="14" t="s">
+      <c r="N20" s="11" t="s">
         <v>78</v>
       </c>
-      <c r="O20" s="14" t="s">
+      <c r="O20" s="11" t="s">
         <v>83</v>
       </c>
     </row>
@@ -1976,10 +2004,10 @@
       <c r="K21" s="2"/>
       <c r="L21" s="2"/>
       <c r="M21" s="2"/>
-      <c r="N21" s="14" t="s">
+      <c r="N21" s="11" t="s">
         <v>78</v>
       </c>
-      <c r="O21" s="14" t="s">
+      <c r="O21" s="11" t="s">
         <v>79</v>
       </c>
     </row>
@@ -2005,7 +2033,7 @@
       <c r="O22" t="s">
         <v>86</v>
       </c>
-      <c r="AI22" s="12"/>
+      <c r="AI22" s="9"/>
       <c r="AJ22" t="s">
         <v>56</v>
       </c>
@@ -2032,7 +2060,7 @@
       <c r="O23" t="s">
         <v>79</v>
       </c>
-      <c r="AI23" s="11"/>
+      <c r="AI23" s="8"/>
       <c r="AJ23" t="s">
         <v>57</v>
       </c>
@@ -2059,7 +2087,7 @@
       <c r="O24" t="s">
         <v>82</v>
       </c>
-      <c r="AI24" s="10"/>
+      <c r="AI24" s="7"/>
       <c r="AJ24" t="s">
         <v>58</v>
       </c>
@@ -2086,7 +2114,7 @@
       <c r="O25" t="s">
         <v>84</v>
       </c>
-      <c r="AI25" s="13"/>
+      <c r="AI25" s="10"/>
       <c r="AJ25" t="s">
         <v>61</v>
       </c>
@@ -2261,4 +2289,166 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{43D97CD3-BA65-40A2-9A26-BFDCD3608E1D}">
+  <dimension ref="B6:O13"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="W23" sqref="W23"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="2" max="18" width="3.7109375" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="6" spans="2:15" x14ac:dyDescent="0.25">
+      <c r="B6" t="s">
+        <v>88</v>
+      </c>
+      <c r="G6">
+        <v>1</v>
+      </c>
+      <c r="H6">
+        <v>2</v>
+      </c>
+      <c r="I6">
+        <v>3</v>
+      </c>
+      <c r="J6">
+        <v>4</v>
+      </c>
+      <c r="K6">
+        <v>5</v>
+      </c>
+      <c r="L6">
+        <v>6</v>
+      </c>
+      <c r="O6" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="7" spans="2:15" x14ac:dyDescent="0.25">
+      <c r="B7">
+        <v>6</v>
+      </c>
+      <c r="C7">
+        <v>3</v>
+      </c>
+      <c r="F7">
+        <v>1</v>
+      </c>
+      <c r="G7" s="15"/>
+      <c r="H7" s="15"/>
+      <c r="I7" s="15"/>
+      <c r="J7" s="15"/>
+      <c r="K7" s="15"/>
+      <c r="L7" s="15"/>
+      <c r="O7" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="8" spans="2:15" x14ac:dyDescent="0.25">
+      <c r="B8">
+        <v>7</v>
+      </c>
+      <c r="C8">
+        <v>6</v>
+      </c>
+      <c r="F8">
+        <v>2</v>
+      </c>
+      <c r="G8" s="15"/>
+      <c r="H8" s="15"/>
+      <c r="I8" s="16"/>
+      <c r="J8" s="17">
+        <v>2</v>
+      </c>
+      <c r="K8" s="17">
+        <v>3</v>
+      </c>
+      <c r="L8" s="15"/>
+      <c r="O8" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="9" spans="2:15" x14ac:dyDescent="0.25">
+      <c r="B9">
+        <v>8</v>
+      </c>
+      <c r="C9">
+        <v>10</v>
+      </c>
+      <c r="F9">
+        <v>3</v>
+      </c>
+      <c r="G9" s="15"/>
+      <c r="H9" s="17">
+        <v>9</v>
+      </c>
+      <c r="I9" s="15"/>
+      <c r="J9" s="17">
+        <v>1</v>
+      </c>
+      <c r="K9" s="17">
+        <v>4</v>
+      </c>
+      <c r="L9" s="15"/>
+    </row>
+    <row r="10" spans="2:15" x14ac:dyDescent="0.25">
+      <c r="F10">
+        <v>4</v>
+      </c>
+      <c r="G10" s="15"/>
+      <c r="H10" s="17">
+        <v>8</v>
+      </c>
+      <c r="I10" s="17">
+        <v>0</v>
+      </c>
+      <c r="J10" s="15"/>
+      <c r="K10" s="17">
+        <v>5</v>
+      </c>
+      <c r="L10" s="15"/>
+      <c r="O10" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="11" spans="2:15" x14ac:dyDescent="0.25">
+      <c r="F11">
+        <v>5</v>
+      </c>
+      <c r="G11" s="15"/>
+      <c r="H11" s="17">
+        <v>7</v>
+      </c>
+      <c r="I11" s="17">
+        <v>6</v>
+      </c>
+      <c r="J11" s="16"/>
+      <c r="K11" s="15"/>
+      <c r="L11" s="15"/>
+    </row>
+    <row r="12" spans="2:15" x14ac:dyDescent="0.25">
+      <c r="F12">
+        <v>6</v>
+      </c>
+      <c r="G12" s="15"/>
+      <c r="H12" s="15"/>
+      <c r="I12" s="15"/>
+      <c r="J12" s="15"/>
+      <c r="K12" s="15"/>
+      <c r="L12" s="15"/>
+    </row>
+    <row r="13" spans="2:15" x14ac:dyDescent="0.25">
+      <c r="B13" t="s">
+        <v>89</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
0.66 prepare for lvl 2 room
</commit_message>
<xml_diff>
--- a/src/main/screeps.xlsx
+++ b/src/main/screeps.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Screeps\screeps-kotlin-starter-master\src\main\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{00AA2DCB-93A5-41AE-8103-F120A96B3372}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0DA7E6AA-00EE-4900-8DB5-F52C8B94B66C}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{E64D4CD0-F693-495E-97B0-F1DF3284CC0F}"/>
   </bookViews>
@@ -32,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="784" uniqueCount="125">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="239" uniqueCount="133">
   <si>
     <t>O</t>
   </si>
@@ -407,6 +407,30 @@
   </si>
   <si>
     <t>snapshot</t>
+  </si>
+  <si>
+    <t>M15</t>
+  </si>
+  <si>
+    <t>M16</t>
+  </si>
+  <si>
+    <t>creep</t>
+  </si>
+  <si>
+    <t>M17</t>
+  </si>
+  <si>
+    <t>M18</t>
+  </si>
+  <si>
+    <t>M19</t>
+  </si>
+  <si>
+    <t>M20</t>
+  </si>
+  <si>
+    <t>M21</t>
   </si>
 </sst>
 </file>
@@ -576,6 +600,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="9" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -585,7 +610,6 @@
     <xf numFmtId="0" fontId="1" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Обычный" xfId="0" builtinId="0"/>
@@ -905,10 +929,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BAF91D9F-DCEA-4E79-967A-CDC2E1F2774F}">
-  <dimension ref="D3:AZ32"/>
+  <dimension ref="D3:AZ31"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="X27" sqref="X27"/>
+      <selection activeCell="U25" sqref="U25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -970,51 +994,51 @@
         <v>6</v>
       </c>
       <c r="Y4" s="2"/>
-      <c r="Z4" s="15" t="s">
+      <c r="Z4" s="16" t="s">
         <v>37</v>
       </c>
-      <c r="AA4" s="16"/>
-      <c r="AB4" s="17"/>
-      <c r="AC4" s="15" t="s">
+      <c r="AA4" s="17"/>
+      <c r="AB4" s="18"/>
+      <c r="AC4" s="16" t="s">
         <v>38</v>
       </c>
-      <c r="AD4" s="16"/>
-      <c r="AE4" s="17"/>
-      <c r="AF4" s="15" t="s">
+      <c r="AD4" s="17"/>
+      <c r="AE4" s="18"/>
+      <c r="AF4" s="16" t="s">
         <v>39</v>
       </c>
-      <c r="AG4" s="16"/>
-      <c r="AH4" s="17"/>
-      <c r="AI4" s="15" t="s">
+      <c r="AG4" s="17"/>
+      <c r="AH4" s="18"/>
+      <c r="AI4" s="16" t="s">
         <v>40</v>
       </c>
-      <c r="AJ4" s="16"/>
-      <c r="AK4" s="17"/>
-      <c r="AL4" s="15" t="s">
+      <c r="AJ4" s="17"/>
+      <c r="AK4" s="18"/>
+      <c r="AL4" s="16" t="s">
         <v>41</v>
       </c>
-      <c r="AM4" s="16"/>
-      <c r="AN4" s="17"/>
-      <c r="AO4" s="15" t="s">
+      <c r="AM4" s="17"/>
+      <c r="AN4" s="18"/>
+      <c r="AO4" s="16" t="s">
         <v>42</v>
       </c>
-      <c r="AP4" s="16"/>
-      <c r="AQ4" s="17"/>
-      <c r="AR4" s="15" t="s">
+      <c r="AP4" s="17"/>
+      <c r="AQ4" s="18"/>
+      <c r="AR4" s="16" t="s">
         <v>43</v>
       </c>
-      <c r="AS4" s="16"/>
-      <c r="AT4" s="17"/>
-      <c r="AU4" s="15" t="s">
+      <c r="AS4" s="17"/>
+      <c r="AT4" s="18"/>
+      <c r="AU4" s="16" t="s">
         <v>44</v>
       </c>
-      <c r="AV4" s="16"/>
-      <c r="AW4" s="17"/>
-      <c r="AX4" s="15" t="s">
+      <c r="AV4" s="17"/>
+      <c r="AW4" s="18"/>
+      <c r="AX4" s="16" t="s">
         <v>45</v>
       </c>
-      <c r="AY4" s="16"/>
-      <c r="AZ4" s="17"/>
+      <c r="AY4" s="17"/>
+      <c r="AZ4" s="18"/>
     </row>
     <row r="5" spans="4:52" x14ac:dyDescent="0.25">
       <c r="D5" t="s">
@@ -2052,36 +2076,62 @@
       <c r="M19" s="2"/>
       <c r="N19" s="14"/>
       <c r="O19" s="14"/>
-      <c r="AI19" s="18"/>
+      <c r="AI19" s="15"/>
       <c r="AJ19" t="s">
         <v>124</v>
       </c>
     </row>
     <row r="20" spans="4:36" x14ac:dyDescent="0.25">
+      <c r="D20" t="s">
+        <v>125</v>
+      </c>
+      <c r="E20" s="2">
+        <v>15</v>
+      </c>
+      <c r="F20" s="2" t="s">
+        <v>59</v>
+      </c>
+      <c r="G20" s="2"/>
+      <c r="H20" s="2"/>
+      <c r="I20" s="2"/>
+      <c r="J20" s="2"/>
+      <c r="K20" s="2"/>
+      <c r="L20" s="2"/>
+      <c r="M20" s="2">
+        <v>1</v>
+      </c>
       <c r="N20" s="14"/>
       <c r="O20" s="14"/>
     </row>
     <row r="21" spans="4:36" x14ac:dyDescent="0.25">
+      <c r="D21" t="s">
+        <v>126</v>
+      </c>
       <c r="E21" s="2"/>
       <c r="F21" s="2" t="s">
-        <v>59</v>
+        <v>82</v>
       </c>
       <c r="G21" s="2"/>
       <c r="H21" s="2"/>
       <c r="I21" s="2"/>
       <c r="J21" s="2"/>
-      <c r="K21" s="2"/>
+      <c r="K21" s="2">
+        <v>1</v>
+      </c>
       <c r="L21" s="2"/>
-      <c r="M21" s="2">
-        <v>1</v>
-      </c>
-      <c r="N21" s="14"/>
+      <c r="M21" s="2"/>
+      <c r="N21" s="14" t="s">
+        <v>127</v>
+      </c>
       <c r="O21" s="14"/>
     </row>
     <row r="22" spans="4:36" x14ac:dyDescent="0.25">
+      <c r="D22" t="s">
+        <v>128</v>
+      </c>
       <c r="E22" s="3"/>
       <c r="F22" s="3" t="s">
-        <v>68</v>
+        <v>72</v>
       </c>
       <c r="G22" s="3"/>
       <c r="H22" s="3">
@@ -2092,7 +2142,9 @@
       <c r="K22" s="3"/>
       <c r="L22" s="3"/>
       <c r="M22" s="3"/>
-      <c r="N22" s="14"/>
+      <c r="N22" s="14" t="s">
+        <v>127</v>
+      </c>
       <c r="O22" s="14"/>
       <c r="AI22" s="9"/>
       <c r="AJ22" t="s">
@@ -2100,20 +2152,25 @@
       </c>
     </row>
     <row r="23" spans="4:36" x14ac:dyDescent="0.25">
-      <c r="E23" s="2"/>
-      <c r="F23" s="2" t="s">
-        <v>69</v>
-      </c>
-      <c r="G23" s="2">
-        <v>1</v>
-      </c>
-      <c r="H23" s="2"/>
-      <c r="I23" s="2"/>
-      <c r="J23" s="2"/>
-      <c r="K23" s="2"/>
-      <c r="L23" s="2"/>
-      <c r="M23" s="2"/>
-      <c r="N23" s="14"/>
+      <c r="D23" t="s">
+        <v>129</v>
+      </c>
+      <c r="E23" s="3"/>
+      <c r="F23" s="3" t="s">
+        <v>80</v>
+      </c>
+      <c r="G23" s="3"/>
+      <c r="H23" s="3"/>
+      <c r="I23" s="3"/>
+      <c r="J23" s="3"/>
+      <c r="K23" s="3">
+        <v>1</v>
+      </c>
+      <c r="L23" s="3"/>
+      <c r="M23" s="3"/>
+      <c r="N23" s="14" t="s">
+        <v>127</v>
+      </c>
       <c r="O23" s="14"/>
       <c r="AI23" s="8"/>
       <c r="AJ23" t="s">
@@ -2121,20 +2178,25 @@
       </c>
     </row>
     <row r="24" spans="4:36" x14ac:dyDescent="0.25">
+      <c r="D24" t="s">
+        <v>130</v>
+      </c>
       <c r="E24" s="3"/>
       <c r="F24" s="3" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="G24" s="3"/>
-      <c r="H24" s="3"/>
+      <c r="H24" s="3">
+        <v>1</v>
+      </c>
       <c r="I24" s="3"/>
-      <c r="J24" s="3">
-        <v>1</v>
-      </c>
+      <c r="J24" s="3"/>
       <c r="K24" s="3"/>
       <c r="L24" s="3"/>
       <c r="M24" s="3"/>
-      <c r="N24" s="14"/>
+      <c r="N24" s="14" t="s">
+        <v>127</v>
+      </c>
       <c r="O24" s="14"/>
       <c r="AI24" s="7"/>
       <c r="AJ24" t="s">
@@ -2142,20 +2204,25 @@
       </c>
     </row>
     <row r="25" spans="4:36" x14ac:dyDescent="0.25">
+      <c r="D25" t="s">
+        <v>131</v>
+      </c>
       <c r="E25" s="2"/>
       <c r="F25" s="2" t="s">
-        <v>82</v>
-      </c>
-      <c r="G25" s="2"/>
+        <v>69</v>
+      </c>
+      <c r="G25" s="2">
+        <v>1</v>
+      </c>
       <c r="H25" s="2"/>
       <c r="I25" s="2"/>
       <c r="J25" s="2"/>
-      <c r="K25" s="2">
-        <v>1</v>
-      </c>
+      <c r="K25" s="2"/>
       <c r="L25" s="2"/>
       <c r="M25" s="2"/>
-      <c r="N25" s="14"/>
+      <c r="N25" s="14" t="s">
+        <v>127</v>
+      </c>
       <c r="O25" s="14"/>
       <c r="AI25" s="10"/>
       <c r="AJ25" t="s">
@@ -2163,144 +2230,134 @@
       </c>
     </row>
     <row r="26" spans="4:36" x14ac:dyDescent="0.25">
+      <c r="D26" t="s">
+        <v>132</v>
+      </c>
       <c r="E26" s="3"/>
       <c r="F26" s="3" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="G26" s="3"/>
-      <c r="H26" s="3">
-        <v>1</v>
-      </c>
+      <c r="H26" s="3"/>
       <c r="I26" s="3"/>
-      <c r="J26" s="3"/>
+      <c r="J26" s="3">
+        <v>1</v>
+      </c>
       <c r="K26" s="3"/>
       <c r="L26" s="3"/>
       <c r="M26" s="3"/>
-      <c r="N26" s="14"/>
+      <c r="N26" s="14" t="s">
+        <v>127</v>
+      </c>
       <c r="O26" s="14"/>
     </row>
     <row r="27" spans="4:36" x14ac:dyDescent="0.25">
-      <c r="E27" s="3"/>
-      <c r="F27" s="3" t="s">
-        <v>80</v>
-      </c>
-      <c r="G27" s="3"/>
-      <c r="H27" s="3"/>
-      <c r="I27" s="3"/>
-      <c r="J27" s="3"/>
-      <c r="K27" s="3">
-        <v>1</v>
-      </c>
-      <c r="L27" s="3"/>
-      <c r="M27" s="3"/>
+      <c r="E27" s="2" t="s">
+        <v>55</v>
+      </c>
+      <c r="F27" s="2"/>
+      <c r="G27" s="2">
+        <v>1</v>
+      </c>
+      <c r="H27" s="2"/>
+      <c r="I27" s="2">
+        <v>2</v>
+      </c>
+      <c r="J27" s="2"/>
+      <c r="K27" s="2">
+        <v>1</v>
+      </c>
+      <c r="L27" s="2"/>
+      <c r="M27" s="2"/>
       <c r="N27" s="14"/>
       <c r="O27" s="14"/>
     </row>
     <row r="28" spans="4:36" x14ac:dyDescent="0.25">
-      <c r="E28" s="2" t="s">
-        <v>55</v>
-      </c>
-      <c r="F28" s="2"/>
-      <c r="G28" s="2">
-        <v>1</v>
-      </c>
-      <c r="H28" s="2"/>
-      <c r="I28" s="2">
-        <v>2</v>
-      </c>
-      <c r="J28" s="2"/>
-      <c r="K28" s="2">
-        <v>1</v>
-      </c>
-      <c r="L28" s="2"/>
-      <c r="M28" s="2"/>
-    </row>
-    <row r="29" spans="4:36" x14ac:dyDescent="0.25">
-      <c r="G29" s="1">
-        <f>SUM(G5:G28)</f>
+      <c r="G28" s="1">
+        <f t="shared" ref="G28:L28" si="0">SUM(G5:G27)</f>
         <v>7</v>
       </c>
-      <c r="H29" s="1">
-        <f>SUM(H5:H28)</f>
+      <c r="H28" s="1">
+        <f t="shared" si="0"/>
         <v>5</v>
       </c>
-      <c r="I29" s="1">
-        <f>SUM(I5:I28)</f>
+      <c r="I28" s="1">
+        <f t="shared" si="0"/>
         <v>4</v>
       </c>
-      <c r="J29" s="1">
-        <f>SUM(J5:J28)</f>
-        <v>1</v>
-      </c>
-      <c r="K29" s="1">
-        <f>SUM(K5:K28)</f>
+      <c r="J28" s="1">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+      <c r="K28" s="1">
+        <f t="shared" si="0"/>
         <v>3</v>
       </c>
-      <c r="L29" s="1">
-        <f>SUM(L5:L28)</f>
+      <c r="L28" s="1">
+        <f t="shared" si="0"/>
         <v>5</v>
       </c>
-      <c r="M29" s="1">
-        <f>SUM(M5:M28)</f>
-        <v>1</v>
+      <c r="M28" s="1">
+        <f>SUM(M5:M27)</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="30" spans="4:36" x14ac:dyDescent="0.25">
+      <c r="F30" t="s">
+        <v>34</v>
+      </c>
+      <c r="G30" s="1">
+        <v>7</v>
+      </c>
+      <c r="H30" s="1">
+        <v>7</v>
+      </c>
+      <c r="I30" s="1">
+        <v>3</v>
+      </c>
+      <c r="J30" s="1">
+        <v>3</v>
+      </c>
+      <c r="K30" s="1">
+        <v>2</v>
+      </c>
+      <c r="L30" s="1">
+        <v>3</v>
+      </c>
+      <c r="M30" s="1">
+        <v>2</v>
       </c>
     </row>
     <row r="31" spans="4:36" x14ac:dyDescent="0.25">
       <c r="F31" t="s">
-        <v>34</v>
-      </c>
-      <c r="G31" s="1">
-        <v>7</v>
-      </c>
-      <c r="H31" s="1">
-        <v>7</v>
-      </c>
-      <c r="I31" s="1">
-        <v>3</v>
-      </c>
-      <c r="J31" s="1">
-        <v>3</v>
-      </c>
-      <c r="K31" s="1">
-        <v>2</v>
-      </c>
-      <c r="L31" s="1">
-        <v>3</v>
-      </c>
-      <c r="M31" s="1">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="32" spans="4:36" x14ac:dyDescent="0.25">
-      <c r="F32" t="s">
         <v>35</v>
       </c>
-      <c r="G32">
-        <f>G31-G29</f>
+      <c r="G31">
+        <f>G30-G28</f>
         <v>0</v>
       </c>
-      <c r="H32">
-        <f t="shared" ref="H32:M32" si="0">H31-H29</f>
-        <v>2</v>
-      </c>
-      <c r="I32">
-        <f t="shared" si="0"/>
+      <c r="H31">
+        <f t="shared" ref="H31:M31" si="1">H30-H28</f>
+        <v>2</v>
+      </c>
+      <c r="I31">
+        <f t="shared" si="1"/>
         <v>-1</v>
       </c>
-      <c r="J32">
-        <f t="shared" si="0"/>
-        <v>2</v>
-      </c>
-      <c r="K32">
-        <f t="shared" si="0"/>
+      <c r="J31">
+        <f t="shared" si="1"/>
+        <v>2</v>
+      </c>
+      <c r="K31">
+        <f t="shared" si="1"/>
         <v>-1</v>
       </c>
-      <c r="L32">
-        <f t="shared" si="0"/>
+      <c r="L31">
+        <f t="shared" si="1"/>
         <v>-2</v>
       </c>
-      <c r="M32">
-        <f t="shared" si="0"/>
+      <c r="M31">
+        <f t="shared" si="1"/>
         <v>1</v>
       </c>
     </row>

</xml_diff>

<commit_message>
0.72 lvl 2 room start develop
</commit_message>
<xml_diff>
--- a/src/main/screeps.xlsx
+++ b/src/main/screeps.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Screeps\screeps-kotlin-starter-master\src\main\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B095390C-FCAA-4935-AB6B-CAD3E60AEE4F}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F7338CDD-8DE3-4800-967F-6BD49838663E}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{E64D4CD0-F693-495E-97B0-F1DF3284CC0F}"/>
   </bookViews>
@@ -954,7 +954,7 @@
   <dimension ref="D3:AZ31"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="AW22" sqref="AW22"/>
+      <selection activeCell="AR22" sqref="AR22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1853,22 +1853,22 @@
       <c r="AL12" s="5"/>
       <c r="AM12" s="5"/>
       <c r="AN12" s="5"/>
-      <c r="AO12" s="10">
-        <v>1</v>
-      </c>
-      <c r="AP12" s="10" t="s">
+      <c r="AO12" s="8">
+        <v>1</v>
+      </c>
+      <c r="AP12" s="8" t="s">
         <v>5</v>
       </c>
-      <c r="AQ12" s="10" t="s">
+      <c r="AQ12" s="8" t="s">
         <v>61</v>
       </c>
-      <c r="AR12" s="7">
-        <v>2</v>
-      </c>
-      <c r="AS12" s="7" t="s">
+      <c r="AR12" s="9">
+        <v>2</v>
+      </c>
+      <c r="AS12" s="9" t="s">
         <v>4</v>
       </c>
-      <c r="AT12" s="7" t="s">
+      <c r="AT12" s="9" t="s">
         <v>67</v>
       </c>
       <c r="AU12" s="5"/>

</xml_diff>

<commit_message>
0.80 lvl 2 room in test, terminal sent in test
</commit_message>
<xml_diff>
--- a/src/main/screeps.xlsx
+++ b/src/main/screeps.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Screeps\screeps-kotlin-starter-master\src\main\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F7338CDD-8DE3-4800-967F-6BD49838663E}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{31FB143C-77A2-4598-9A13-E7B394BAC0DD}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{E64D4CD0-F693-495E-97B0-F1DF3284CC0F}"/>
   </bookViews>
@@ -1275,7 +1275,7 @@
       <c r="AT6" s="10" t="s">
         <v>62</v>
       </c>
-      <c r="AU6" s="8">
+      <c r="AU6" s="15">
         <v>1</v>
       </c>
       <c r="AV6" s="8" t="s">
@@ -1665,7 +1665,7 @@
       <c r="Y10" s="2" t="s">
         <v>51</v>
       </c>
-      <c r="Z10" s="8">
+      <c r="Z10" s="15">
         <v>1</v>
       </c>
       <c r="AA10" s="8" t="s">
@@ -1784,13 +1784,13 @@
       <c r="AL11" s="5"/>
       <c r="AM11" s="5"/>
       <c r="AN11" s="5"/>
-      <c r="AO11" s="10">
-        <v>1</v>
-      </c>
-      <c r="AP11" s="10" t="s">
+      <c r="AO11" s="15">
+        <v>1</v>
+      </c>
+      <c r="AP11" s="8" t="s">
         <v>0</v>
       </c>
-      <c r="AQ11" s="10" t="s">
+      <c r="AQ11" s="8" t="s">
         <v>61</v>
       </c>
       <c r="AR11" s="10">

</xml_diff>

<commit_message>
0.81 market buy energy
</commit_message>
<xml_diff>
--- a/src/main/screeps.xlsx
+++ b/src/main/screeps.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Screeps\screeps-kotlin-starter-master\src\main\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{31FB143C-77A2-4598-9A13-E7B394BAC0DD}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FEA3C242-C669-43C3-B274-AB54CEF09EC0}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{E64D4CD0-F693-495E-97B0-F1DF3284CC0F}"/>
   </bookViews>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="247" uniqueCount="140">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="248" uniqueCount="142">
   <si>
     <t>O</t>
   </si>
@@ -453,6 +453,12 @@
   </si>
   <si>
     <t>ticks per hour</t>
+  </si>
+  <si>
+    <t>2 lvl snapshot</t>
+  </si>
+  <si>
+    <t>M06</t>
   </si>
 </sst>
 </file>
@@ -484,7 +490,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="10">
+  <fills count="11">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -536,6 +542,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="-0.499984740745262"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -604,7 +616,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="19">
+  <cellXfs count="21">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
@@ -632,6 +644,8 @@
     <xf numFmtId="0" fontId="1" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="10" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="10" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Обычный" xfId="0" builtinId="0"/>
@@ -954,7 +968,7 @@
   <dimension ref="D3:AZ31"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="AR22" sqref="AR22"/>
+      <selection activeCell="AR25" sqref="AR25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1114,13 +1128,13 @@
       <c r="AB5" s="9" t="s">
         <v>63</v>
       </c>
-      <c r="AC5" s="6">
-        <v>1</v>
-      </c>
-      <c r="AD5" s="8" t="s">
+      <c r="AC5" s="15">
+        <v>1</v>
+      </c>
+      <c r="AD5" s="15" t="s">
         <v>0</v>
       </c>
-      <c r="AE5" s="8" t="s">
+      <c r="AE5" s="15" t="s">
         <v>61</v>
       </c>
       <c r="AF5" s="9">
@@ -1132,15 +1146,13 @@
       <c r="AH5" s="9" t="s">
         <v>63</v>
       </c>
-      <c r="AI5" s="9">
-        <v>2</v>
-      </c>
-      <c r="AJ5" s="9" t="s">
-        <v>2</v>
-      </c>
-      <c r="AK5" s="9" t="s">
-        <v>63</v>
-      </c>
+      <c r="AI5" s="19" t="s">
+        <v>141</v>
+      </c>
+      <c r="AJ5" s="19" t="s">
+        <v>2</v>
+      </c>
+      <c r="AK5" s="19"/>
       <c r="AL5" s="5"/>
       <c r="AM5" s="5"/>
       <c r="AN5" s="5"/>
@@ -1153,29 +1165,29 @@
       <c r="AQ5" s="10" t="s">
         <v>61</v>
       </c>
-      <c r="AR5" s="7">
-        <v>1</v>
-      </c>
-      <c r="AS5" s="7" t="s">
+      <c r="AR5" s="9">
+        <v>1</v>
+      </c>
+      <c r="AS5" s="9" t="s">
         <v>4</v>
       </c>
-      <c r="AT5" s="7" t="s">
+      <c r="AT5" s="9" t="s">
         <v>67</v>
       </c>
-      <c r="AU5" s="7">
-        <v>1</v>
-      </c>
-      <c r="AV5" s="7" t="s">
-        <v>2</v>
-      </c>
-      <c r="AW5" s="7"/>
-      <c r="AX5" s="6">
-        <v>1</v>
-      </c>
-      <c r="AY5" s="8" t="s">
-        <v>1</v>
-      </c>
-      <c r="AZ5" s="8" t="s">
+      <c r="AU5" s="9">
+        <v>1</v>
+      </c>
+      <c r="AV5" s="9" t="s">
+        <v>2</v>
+      </c>
+      <c r="AW5" s="9"/>
+      <c r="AX5" s="15">
+        <v>1</v>
+      </c>
+      <c r="AY5" s="15" t="s">
+        <v>1</v>
+      </c>
+      <c r="AZ5" s="15" t="s">
         <v>74</v>
       </c>
     </row>
@@ -1220,13 +1232,13 @@
       <c r="Y6" s="2" t="s">
         <v>47</v>
       </c>
-      <c r="Z6" s="6">
-        <v>1</v>
-      </c>
-      <c r="AA6" s="8" t="s">
+      <c r="Z6" s="15">
+        <v>1</v>
+      </c>
+      <c r="AA6" s="15" t="s">
         <v>5</v>
       </c>
-      <c r="AB6" s="8" t="s">
+      <c r="AB6" s="15" t="s">
         <v>62</v>
       </c>
       <c r="AC6" s="9">
@@ -1278,10 +1290,10 @@
       <c r="AU6" s="15">
         <v>1</v>
       </c>
-      <c r="AV6" s="8" t="s">
+      <c r="AV6" s="15" t="s">
         <v>0</v>
       </c>
-      <c r="AW6" s="8" t="s">
+      <c r="AW6" s="15" t="s">
         <v>74</v>
       </c>
       <c r="AX6" s="9">
@@ -1353,13 +1365,13 @@
       <c r="AE7" s="9" t="s">
         <v>65</v>
       </c>
-      <c r="AF7" s="6">
-        <v>1</v>
-      </c>
-      <c r="AG7" s="8" t="s">
+      <c r="AF7" s="15">
+        <v>1</v>
+      </c>
+      <c r="AG7" s="15" t="s">
         <v>0</v>
       </c>
-      <c r="AH7" s="8" t="s">
+      <c r="AH7" s="15" t="s">
         <v>61</v>
       </c>
       <c r="AI7" s="9">
@@ -1377,13 +1389,13 @@
       <c r="AO7" s="5"/>
       <c r="AP7" s="5"/>
       <c r="AQ7" s="5"/>
-      <c r="AR7" s="7">
-        <v>1</v>
-      </c>
-      <c r="AS7" s="7" t="s">
+      <c r="AR7" s="9">
+        <v>1</v>
+      </c>
+      <c r="AS7" s="9" t="s">
         <v>0</v>
       </c>
-      <c r="AT7" s="7" t="s">
+      <c r="AT7" s="9" t="s">
         <v>64</v>
       </c>
       <c r="AU7" s="9">
@@ -1395,13 +1407,13 @@
       <c r="AW7" s="9" t="s">
         <v>63</v>
       </c>
-      <c r="AX7" s="6">
-        <v>1</v>
-      </c>
-      <c r="AY7" s="8" t="s">
+      <c r="AX7" s="15">
+        <v>1</v>
+      </c>
+      <c r="AY7" s="15" t="s">
         <v>0</v>
       </c>
-      <c r="AZ7" s="8" t="s">
+      <c r="AZ7" s="15" t="s">
         <v>62</v>
       </c>
     </row>
@@ -1450,10 +1462,10 @@
       <c r="Z8" s="15">
         <v>1</v>
       </c>
-      <c r="AA8" s="8" t="s">
+      <c r="AA8" s="15" t="s">
         <v>4</v>
       </c>
-      <c r="AB8" s="8" t="s">
+      <c r="AB8" s="15" t="s">
         <v>61</v>
       </c>
       <c r="AC8" s="9">
@@ -1468,10 +1480,10 @@
       <c r="AF8" s="15">
         <v>1</v>
       </c>
-      <c r="AG8" s="8" t="s">
+      <c r="AG8" s="15" t="s">
         <v>4</v>
       </c>
-      <c r="AH8" s="8" t="s">
+      <c r="AH8" s="15" t="s">
         <v>66</v>
       </c>
       <c r="AI8" s="10">
@@ -1495,22 +1507,22 @@
       <c r="AQ8" s="10" t="s">
         <v>61</v>
       </c>
-      <c r="AR8" s="10">
-        <v>1</v>
-      </c>
-      <c r="AS8" s="10" t="s">
-        <v>2</v>
-      </c>
-      <c r="AT8" s="10" t="s">
+      <c r="AR8" s="15">
+        <v>1</v>
+      </c>
+      <c r="AS8" s="15" t="s">
+        <v>2</v>
+      </c>
+      <c r="AT8" s="15" t="s">
         <v>62</v>
       </c>
-      <c r="AU8" s="6">
-        <v>1</v>
-      </c>
-      <c r="AV8" s="8" t="s">
+      <c r="AU8" s="15">
+        <v>1</v>
+      </c>
+      <c r="AV8" s="15" t="s">
         <v>0</v>
       </c>
-      <c r="AW8" s="8" t="s">
+      <c r="AW8" s="15" t="s">
         <v>61</v>
       </c>
       <c r="AX8" s="9">
@@ -1600,13 +1612,13 @@
       <c r="AQ9" s="10" t="s">
         <v>61</v>
       </c>
-      <c r="AR9" s="7">
-        <v>1</v>
-      </c>
-      <c r="AS9" s="7" t="s">
-        <v>2</v>
-      </c>
-      <c r="AT9" s="7" t="s">
+      <c r="AR9" s="9">
+        <v>1</v>
+      </c>
+      <c r="AS9" s="9" t="s">
+        <v>2</v>
+      </c>
+      <c r="AT9" s="9" t="s">
         <v>67</v>
       </c>
       <c r="AU9" s="10">
@@ -1668,19 +1680,19 @@
       <c r="Z10" s="15">
         <v>1</v>
       </c>
-      <c r="AA10" s="8" t="s">
-        <v>1</v>
-      </c>
-      <c r="AB10" s="8" t="s">
+      <c r="AA10" s="15" t="s">
+        <v>1</v>
+      </c>
+      <c r="AB10" s="15" t="s">
         <v>74</v>
       </c>
-      <c r="AC10" s="6">
-        <v>1</v>
-      </c>
-      <c r="AD10" s="8" t="s">
+      <c r="AC10" s="15">
+        <v>1</v>
+      </c>
+      <c r="AD10" s="15" t="s">
         <v>5</v>
       </c>
-      <c r="AE10" s="8" t="s">
+      <c r="AE10" s="15" t="s">
         <v>62</v>
       </c>
       <c r="AF10" s="5"/>
@@ -1718,7 +1730,7 @@
       <c r="AZ10" s="5"/>
     </row>
     <row r="11" spans="4:52" x14ac:dyDescent="0.25">
-      <c r="D11" t="s">
+      <c r="D11" s="20" t="s">
         <v>94</v>
       </c>
       <c r="E11" s="2">
@@ -1787,19 +1799,19 @@
       <c r="AO11" s="15">
         <v>1</v>
       </c>
-      <c r="AP11" s="8" t="s">
+      <c r="AP11" s="15" t="s">
         <v>0</v>
       </c>
-      <c r="AQ11" s="8" t="s">
+      <c r="AQ11" s="15" t="s">
         <v>61</v>
       </c>
-      <c r="AR11" s="10">
-        <v>2</v>
-      </c>
-      <c r="AS11" s="10" t="s">
+      <c r="AR11" s="15">
+        <v>2</v>
+      </c>
+      <c r="AS11" s="15" t="s">
         <v>0</v>
       </c>
-      <c r="AT11" s="10" t="s">
+      <c r="AT11" s="15" t="s">
         <v>62</v>
       </c>
       <c r="AU11" s="5"/>
@@ -1853,13 +1865,13 @@
       <c r="AL12" s="5"/>
       <c r="AM12" s="5"/>
       <c r="AN12" s="5"/>
-      <c r="AO12" s="8">
-        <v>1</v>
-      </c>
-      <c r="AP12" s="8" t="s">
+      <c r="AO12" s="15">
+        <v>1</v>
+      </c>
+      <c r="AP12" s="15" t="s">
         <v>5</v>
       </c>
-      <c r="AQ12" s="8" t="s">
+      <c r="AQ12" s="15" t="s">
         <v>61</v>
       </c>
       <c r="AR12" s="9">
@@ -1922,22 +1934,22 @@
       <c r="AL13" s="5"/>
       <c r="AM13" s="5"/>
       <c r="AN13" s="5"/>
-      <c r="AO13" s="10">
-        <v>1</v>
-      </c>
-      <c r="AP13" s="10" t="s">
+      <c r="AO13" s="8">
+        <v>1</v>
+      </c>
+      <c r="AP13" s="8" t="s">
         <v>6</v>
       </c>
-      <c r="AQ13" s="10" t="s">
+      <c r="AQ13" s="8" t="s">
         <v>62</v>
       </c>
-      <c r="AR13" s="10">
-        <v>1</v>
-      </c>
-      <c r="AS13" s="10" t="s">
+      <c r="AR13" s="8">
+        <v>1</v>
+      </c>
+      <c r="AS13" s="8" t="s">
         <v>5</v>
       </c>
-      <c r="AT13" s="10" t="s">
+      <c r="AT13" s="8" t="s">
         <v>66</v>
       </c>
       <c r="AU13" s="5"/>
@@ -2028,7 +2040,7 @@
       <c r="U16" s="3"/>
       <c r="V16" s="3"/>
     </row>
-    <row r="17" spans="4:36" x14ac:dyDescent="0.25">
+    <row r="17" spans="4:40" x14ac:dyDescent="0.25">
       <c r="D17" t="s">
         <v>89</v>
       </c>
@@ -2057,7 +2069,7 @@
       <c r="U17" s="2"/>
       <c r="V17" s="2"/>
     </row>
-    <row r="18" spans="4:36" x14ac:dyDescent="0.25">
+    <row r="18" spans="4:40" x14ac:dyDescent="0.25">
       <c r="D18" t="s">
         <v>90</v>
       </c>
@@ -2079,7 +2091,7 @@
       <c r="N18" s="14"/>
       <c r="O18" s="14"/>
     </row>
-    <row r="19" spans="4:36" x14ac:dyDescent="0.25">
+    <row r="19" spans="4:40" x14ac:dyDescent="0.25">
       <c r="D19" t="s">
         <v>123</v>
       </c>
@@ -2104,8 +2116,12 @@
       <c r="AJ19" t="s">
         <v>124</v>
       </c>
-    </row>
-    <row r="20" spans="4:36" x14ac:dyDescent="0.25">
+      <c r="AM19" s="20"/>
+      <c r="AN19" t="s">
+        <v>140</v>
+      </c>
+    </row>
+    <row r="20" spans="4:40" x14ac:dyDescent="0.25">
       <c r="D20" t="s">
         <v>125</v>
       </c>
@@ -2127,7 +2143,7 @@
       <c r="N20" s="14"/>
       <c r="O20" s="14"/>
     </row>
-    <row r="21" spans="4:36" x14ac:dyDescent="0.25">
+    <row r="21" spans="4:40" x14ac:dyDescent="0.25">
       <c r="D21" t="s">
         <v>126</v>
       </c>
@@ -2149,7 +2165,7 @@
       </c>
       <c r="O21" s="14"/>
     </row>
-    <row r="22" spans="4:36" x14ac:dyDescent="0.25">
+    <row r="22" spans="4:40" x14ac:dyDescent="0.25">
       <c r="D22" t="s">
         <v>128</v>
       </c>
@@ -2175,7 +2191,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="23" spans="4:36" x14ac:dyDescent="0.25">
+    <row r="23" spans="4:40" x14ac:dyDescent="0.25">
       <c r="D23" t="s">
         <v>129</v>
       </c>
@@ -2201,7 +2217,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="24" spans="4:36" x14ac:dyDescent="0.25">
+    <row r="24" spans="4:40" x14ac:dyDescent="0.25">
       <c r="D24" t="s">
         <v>130</v>
       </c>
@@ -2227,7 +2243,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="25" spans="4:36" x14ac:dyDescent="0.25">
+    <row r="25" spans="4:40" x14ac:dyDescent="0.25">
       <c r="D25" t="s">
         <v>131</v>
       </c>
@@ -2253,7 +2269,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="26" spans="4:36" x14ac:dyDescent="0.25">
+    <row r="26" spans="4:40" x14ac:dyDescent="0.25">
       <c r="D26" t="s">
         <v>132</v>
       </c>
@@ -2275,7 +2291,7 @@
       </c>
       <c r="O26" s="14"/>
     </row>
-    <row r="27" spans="4:36" x14ac:dyDescent="0.25">
+    <row r="27" spans="4:40" x14ac:dyDescent="0.25">
       <c r="E27" s="2" t="s">
         <v>55</v>
       </c>
@@ -2296,7 +2312,7 @@
       <c r="N27" s="14"/>
       <c r="O27" s="14"/>
     </row>
-    <row r="28" spans="4:36" x14ac:dyDescent="0.25">
+    <row r="28" spans="4:40" x14ac:dyDescent="0.25">
       <c r="G28" s="1">
         <f t="shared" ref="G28:L28" si="0">SUM(G5:G27)</f>
         <v>7</v>
@@ -2326,7 +2342,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="30" spans="4:36" x14ac:dyDescent="0.25">
+    <row r="30" spans="4:40" x14ac:dyDescent="0.25">
       <c r="F30" t="s">
         <v>34</v>
       </c>
@@ -2352,7 +2368,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="31" spans="4:36" x14ac:dyDescent="0.25">
+    <row r="31" spans="4:40" x14ac:dyDescent="0.25">
       <c r="F31" t="s">
         <v>35</v>
       </c>
@@ -2880,13 +2896,16 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{98482179-5758-4672-AADB-0AB0285AA3CF}">
-  <dimension ref="E4:J16"/>
+  <dimension ref="E4:M25"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="I18" sqref="I18"/>
+      <selection activeCell="M30" sqref="M30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="13" max="13" width="10" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="4" spans="5:10" x14ac:dyDescent="0.25">
       <c r="G4" t="s">
@@ -2960,6 +2979,12 @@
         <v>444342.85714285722</v>
       </c>
     </row>
+    <row r="25" spans="13:13" x14ac:dyDescent="0.25">
+      <c r="M25">
+        <f>1263000/0.012</f>
+        <v>105250000</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>